<commit_message>
Fix and Rerun SCD0210, SCD0215, SCD0216, SCD0217, and SCD0218
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0017 - Upload List File Expired 1 Bulan.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0017 - Upload List File Expired 1 Bulan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF512EA7-2776-4F7D-B53E-520625365740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89D69FF-DC53-4751-AF6A-138B59FC8FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9AD3C288-A382-489C-B5A3-5612378D2CD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9AD3C288-A382-489C-B5A3-5612378D2CD7}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0017" sheetId="1" r:id="rId1"/>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BE5456-1E7C-409D-93CC-40083DA405EA}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +831,7 @@
       </c>
       <c r="S4" s="5" t="str">
         <f ca="1">"USE DigisalesNew; UPDATE dbo.MasterFile SET ExpiredDate = '"&amp;TEXT(TODAY()-31,"yyyy-mm-dd")&amp;"' WHERE keterangan = '"&amp;N2&amp;"'"</f>
-        <v>USE DigisalesNew; UPDATE dbo.MasterFile SET ExpiredDate = '2022-06-04' WHERE keterangan = 'Testing UFT SCD0017'</v>
+        <v>USE DigisalesNew; UPDATE dbo.MasterFile SET ExpiredDate = '2022-07-03' WHERE keterangan = 'Testing UFT SCD0017'</v>
       </c>
       <c r="T4" s="4"/>
       <c r="U4" s="4" t="str">

</xml_diff>